<commit_message>
Implemented logic to get trails from the database and show on frontend
</commit_message>
<xml_diff>
--- a/csc473_project/constant/trails.xlsx
+++ b/csc473_project/constant/trails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nissansunar/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F2CF86-9163-1D40-8CA5-F0AE66112A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5051C152-57F1-C947-A218-623AA13337D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="660" windowWidth="33600" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="271">
   <si>
     <t>ID001</t>
   </si>
@@ -37,9 +37,6 @@
     <t>A legendary trail spanning 2,190 miles from Georgia to Maine.</t>
   </si>
   <si>
-    <t>Georgia to Maine</t>
-  </si>
-  <si>
     <t>https://appalachiantrail.org/wp-content/uploads/2020/02/ATC_RP13443_DSC_5916-2-lpr-1200x800.jpg</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>A challenging trail from Mexico to Canada, crossing diverse landscapes.</t>
   </si>
   <si>
-    <t>California, Oregon, Washington</t>
-  </si>
-  <si>
     <t>https://images.seattletimes.com/wp-content/uploads/2016/07/5f2d7148-4492-11e6-a743-3c8e8a4b2f7a.jpg?d=2040x1302</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>Located in California, passing through Yosemite and Kings Canyon.</t>
   </si>
   <si>
-    <t>California</t>
-  </si>
-  <si>
     <t>https://symg.com/wp-content/uploads/2022/11/NorthboundHEROfinalTINY.jpg</t>
   </si>
   <si>
@@ -94,9 +85,6 @@
     <t>Known for its steep drop-offs and thrilling vistas in Zion National Park.</t>
   </si>
   <si>
-    <t>Utah</t>
-  </si>
-  <si>
     <t>https://www.citrusmilo.com/zion2012/joebraun_angelslanding02.jpg</t>
   </si>
   <si>
@@ -127,9 +115,6 @@
     <t>Descends into the Grand Canyon, offering spectacular canyon views.</t>
   </si>
   <si>
-    <t>Arizona</t>
-  </si>
-  <si>
     <t>https://www.nps.gov/common/uploads/cropped_image/primary/3CF1FA2F-F5C3-E839-3CE0746FFE55B295.jpg?width=1600&amp;quality=90&amp;mode=crop</t>
   </si>
   <si>
@@ -163,9 +148,6 @@
     <t>A rugged coastal trail along the Nā Pali Coast in Hawaii.</t>
   </si>
   <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
     <t>https://images.squarespace-cdn.com/content/v1/58ddd25a15d5db2b31d11726/e8078469-716b-474c-993c-9d00e2210562/Lily-Tang-Kalalau-Trail-Napali-Coast-Kauai-7790.jpg</t>
   </si>
   <si>
@@ -181,9 +163,6 @@
     <t>A panoramic loop in the White Mountains of New Hampshire.</t>
   </si>
   <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
     <t>https://hikingproject.com/assets/photos/hike/7018044_medium_1554830264.jpg?cache=1731132403</t>
   </si>
   <si>
@@ -214,9 +193,6 @@
     <t>Maine's highest peak, offering an adventurous and scenic climb.</t>
   </si>
   <si>
-    <t>Maine</t>
-  </si>
-  <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcR-ne7dZkN4_mJuX1L1QAo3mHqHRsqFmwUBpQ&amp;s</t>
   </si>
   <si>
@@ -247,9 +223,6 @@
     <t>A spectacular trail in Glacier National Park with alpine views.</t>
   </si>
   <si>
-    <t>Montana</t>
-  </si>
-  <si>
     <t>https://glacierguides.com/wp-content/uploads/525172B8-3F15-4482-9124-F24A2C45165D-scaled-e1653764363794.jpg</t>
   </si>
   <si>
@@ -265,9 +238,6 @@
     <t>Traverses Grand Teton National Park with unparalleled mountain scenery.</t>
   </si>
   <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
     <t>https://www.cleverhiker.com/wp-content/uploads/2024/05/image-251.jpeg</t>
   </si>
   <si>
@@ -283,9 +253,6 @@
     <t>Spanning 3,100 miles along the Continental Divide in the Rockies.</t>
   </si>
   <si>
-    <t>New Mexico to Montana</t>
-  </si>
-  <si>
     <t>https://images.squarespace-cdn.com/content/v1/6513fec59a2356315a19625a/1695810369623-07K1XKLLWBK5VQQ5XSS8/shutterstock_1484203367-scaled.jpg</t>
   </si>
   <si>
@@ -301,9 +268,6 @@
     <t>Provides views of Mount Rainier and surrounding meadows in Washington.</t>
   </si>
   <si>
-    <t>Washington</t>
-  </si>
-  <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTTdL8QbGhOSSHen90uApPR5uEcomEfES1o_A&amp;s</t>
   </si>
   <si>
@@ -319,9 +283,6 @@
     <t>Leads to the Harding Icefield with views of expansive Alaskan glaciers.</t>
   </si>
   <si>
-    <t>Alaska</t>
-  </si>
-  <si>
     <t>https://www.nps.gov/kefj/planyourvisit/images/Harding-Icefield-Fiona-RD-255pix_1.jpg</t>
   </si>
   <si>
@@ -337,9 +298,6 @@
     <t>A strenuous route to Longs Peak's summit in Rocky Mountain National Park.</t>
   </si>
   <si>
-    <t>Colorado</t>
-  </si>
-  <si>
     <t>https://www.alanarnette.com/images/Longs%20Peak/routes/keyhole/IMG_0746-1.JPG</t>
   </si>
   <si>
@@ -355,9 +313,6 @@
     <t>Traverses the Ozark National Forest, featuring waterfalls and bluffs.</t>
   </si>
   <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/miles-extranet-dev/image/upload/w_800,h_480,c_fill/Arkansas/account_photos/5098/96f9f2135775ca076f7f6d93b65b23ca_Untitled-1_0000_resize_0008_OzarkHighlandsTrail</t>
   </si>
   <si>
@@ -373,9 +328,6 @@
     <t>Follows Lake Superior's ridgeline, offering sweeping lake views.</t>
   </si>
   <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
     <t>https://media.wildernessinquiry.org/itinerary/superior-hiking-trail-lodge-based-exploration/featured/superior-hiking-trail-lodge-based-exploration-1600x690.jpg</t>
   </si>
   <si>
@@ -391,9 +343,6 @@
     <t>A challenging loop in Pennsylvania's wilderness with dramatic vistas.</t>
   </si>
   <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/3/37/Black_Forest_Trail_Drop-Off.jpg</t>
   </si>
   <si>
@@ -424,9 +373,6 @@
     <t>A coastal trail on Vancouver Island with rainforest and ocean scenery.</t>
   </si>
   <si>
-    <t>British Columbia</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/45/Flat_section_close_to_Sombrio_Point%2C_Juan_de_Fuca_Trail%2C_Vancouver_Island%2C_Canada_13.jpg/1200px-Flat_section_close_to_Sombrio_Point%2C_Juan_de_Fuca_Trail%2C_Vancouver_Island%2C_Canada_13.jpg</t>
   </si>
   <si>
@@ -442,9 +388,6 @@
     <t>A lesser-known Appalachian trail with remote and tranquil landscapes.</t>
   </si>
   <si>
-    <t>Georgia to North Carolina</t>
-  </si>
-  <si>
     <t>https://bmta.org/wp-content/uploads/2020/01/hero.jpg</t>
   </si>
   <si>
@@ -460,9 +403,6 @@
     <t>A long-distance trail highlighting Wisconsin's glacial landscapes.</t>
   </si>
   <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
     <t>https://www.iceagetrail.org/wp-content/uploads/wisconsin-ice-age-trail-view-of-the-bluff-scaled.jpg</t>
   </si>
   <si>
@@ -475,9 +415,6 @@
     <t>Encircles Lake Tahoe with scenic alpine views.</t>
   </si>
   <si>
-    <t>California, Nevada</t>
-  </si>
-  <si>
     <t>https://doingmiles.com/wp-content/uploads/2018/10/2018.10-tahoe-rim-trail-1-feature.jpg</t>
   </si>
   <si>
@@ -493,9 +430,6 @@
     <t>A popular and challenging loop on Old Rag Mountain in Virginia.</t>
   </si>
   <si>
-    <t>Virginia</t>
-  </si>
-  <si>
     <t>https://www.nps.gov/common/uploads/cropped_image/primary/827699E5-94E1-A320-CEB9F6FC0A97FB6C.jpg?width=1600&amp;quality=90&amp;mode=crop</t>
   </si>
   <si>
@@ -565,9 +499,6 @@
     <t>A steep climb offering views of Cascade Pass in the North Cascades.</t>
   </si>
   <si>
-    <t>Oregon</t>
-  </si>
-  <si>
     <t>https://www.nps.gov/noca/planyourvisit/images/NOCA-2012-Resting_Together-Dixon.jpg</t>
   </si>
   <si>
@@ -580,9 +511,6 @@
     <t>Encircles Mount Hood with dramatic views and diverse ecosystems.</t>
   </si>
   <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
     <t>https://cdn.backpacker.com/wp-content/uploads/2019/07/bp0819play_ll_timberlinepp6be4_bjk.jpg</t>
   </si>
   <si>
@@ -628,9 +556,6 @@
     <t>Provides breathtaking views of the Grand Canyon from South Kaibab Trail.</t>
   </si>
   <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
     <t>https://www.nps.gov/common/uploads/cropped_image/primary/B4E27A94-95C8-0019-58893581D89DFCBD.jpg?width=1600&amp;quality=90&amp;mode=crop</t>
   </si>
   <si>
@@ -733,9 +658,6 @@
     <t>Scenic views and wooded trails in the Blue Ridge Mountains.</t>
   </si>
   <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRLWsQzRtyuylJ-ylqD3pr8mlYoi-okjyEWbg&amp;s</t>
   </si>
   <si>
@@ -817,9 +739,6 @@
     <t>A forested trail leading to Carbon Glacier in Mount Rainier National Park.</t>
   </si>
   <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
     <t>https://www.nps.gov/common/uploads/cropped_image/primary/11EE6E1B-9038-94B8-9DC1A7178E78DD8D.jpeg?width=1600&amp;quality=90&amp;mode=crop</t>
   </si>
   <si>
@@ -842,6 +761,78 @@
   </si>
   <si>
     <t>image_url</t>
+  </si>
+  <si>
+    <t>georgia</t>
+  </si>
+  <si>
+    <t>california</t>
+  </si>
+  <si>
+    <t>utah</t>
+  </si>
+  <si>
+    <t>arizona</t>
+  </si>
+  <si>
+    <t>hawaii</t>
+  </si>
+  <si>
+    <t>new hampshire</t>
+  </si>
+  <si>
+    <t>maine</t>
+  </si>
+  <si>
+    <t>montana</t>
+  </si>
+  <si>
+    <t>wyoming</t>
+  </si>
+  <si>
+    <t>new mexico</t>
+  </si>
+  <si>
+    <t>washington</t>
+  </si>
+  <si>
+    <t>alaska</t>
+  </si>
+  <si>
+    <t>colorado</t>
+  </si>
+  <si>
+    <t>arkansas</t>
+  </si>
+  <si>
+    <t>minnesota</t>
+  </si>
+  <si>
+    <t>pennsylvania</t>
+  </si>
+  <si>
+    <t>british columbia</t>
+  </si>
+  <si>
+    <t>wisconsin</t>
+  </si>
+  <si>
+    <t>virginia</t>
+  </si>
+  <si>
+    <t>oregon</t>
+  </si>
+  <si>
+    <t>kentucky</t>
+  </si>
+  <si>
+    <t>north carolina</t>
+  </si>
+  <si>
+    <t>tennessee</t>
+  </si>
+  <si>
+    <t>south dakota</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1168,31 +1159,31 @@
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="67.5" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" customWidth="1"/>
-    <col min="7" max="7" width="96.33203125" customWidth="1"/>
+    <col min="7" max="7" width="217.5" customWidth="1"/>
     <col min="8" max="25" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1212,1137 +1203,1137 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>251</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>252</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>18</v>
+        <v>248</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>75</v>
+        <v>254</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>81</v>
+        <v>255</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>87</v>
+        <v>256</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>99</v>
+        <v>258</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>105</v>
+        <v>259</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>111</v>
+        <v>260</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>117</v>
+        <v>261</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>134</v>
+        <v>263</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>140</v>
+        <v>247</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>146</v>
+        <v>264</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>151</v>
+        <v>248</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>157</v>
+        <v>265</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>181</v>
+        <v>266</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>186</v>
+        <v>267</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>105</v>
+        <v>259</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>202</v>
+        <v>268</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>18</v>
+        <v>248</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>202</v>
+        <v>268</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>53</v>
+        <v>252</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>53</v>
+        <v>252</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>53</v>
+        <v>252</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="G50" s="3" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>